<commit_message>
added shear and negative flexure to lrfr class
</commit_message>
<xml_diff>
--- a/docs/templates/LRFR_Template_v2.xlsx
+++ b/docs/templates/LRFR_Template_v2.xlsx
@@ -15,8 +15,9 @@
     <sheet name="LRFR - Responses - Shear" sheetId="5" r:id="rId6"/>
     <sheet name="LRFR - Ratings - Shear" sheetId="9" r:id="rId7"/>
     <sheet name="Rating Factors" sheetId="12" r:id="rId8"/>
-    <sheet name="API Info" sheetId="14" r:id="rId9"/>
+    <sheet name="Settings" sheetId="14" r:id="rId9"/>
     <sheet name="tmp" sheetId="15" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -122,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="172">
   <si>
     <t>INSERT SCREENSHOTS OF RELEVANT PLANS HERE</t>
   </si>
@@ -337,9 +338,6 @@
     <t>LRFR Shear Capacity</t>
   </si>
   <si>
-    <t>LRFR FLEXURE RESPONSES</t>
-  </si>
-  <si>
     <t>Calculated Total Fiber [psi]</t>
   </si>
   <si>
@@ -379,9 +377,6 @@
     <t>Type 3-3 75%</t>
   </si>
   <si>
-    <t>LRFR SHEAR RESPONSES</t>
-  </si>
-  <si>
     <t>Extracted Shear Responses, FZ [lb]</t>
   </si>
   <si>
@@ -448,12 +443,6 @@
     <t>Service II Operating</t>
   </si>
   <si>
-    <t>LRFR FLEXURE RATINGS</t>
-  </si>
-  <si>
-    <t>LRFR SHEAR RATINGS</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
@@ -472,9 +461,6 @@
     <t>Calculated Composite Moment [lb-in]</t>
   </si>
   <si>
-    <t>Template Version</t>
-  </si>
-  <si>
     <t>[int]</t>
   </si>
   <si>
@@ -611,6 +597,48 @@
   </si>
   <si>
     <t>wSDW</t>
+  </si>
+  <si>
+    <t>Positive Region (Near)</t>
+  </si>
+  <si>
+    <t>Beam #</t>
+  </si>
+  <si>
+    <t>Beam End</t>
+  </si>
+  <si>
+    <t>Shell #</t>
+  </si>
+  <si>
+    <t>* Output only tab</t>
+  </si>
+  <si>
+    <t>[interior/exterior]</t>
+  </si>
+  <si>
+    <t>[interior/end]</t>
+  </si>
+  <si>
+    <t>Transverse Location</t>
+  </si>
+  <si>
+    <t>Shear Panel Location</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>model</t>
   </si>
 </sst>
 </file>
@@ -675,19 +703,10 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -764,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -799,29 +818,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -846,21 +864,38 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -874,16 +909,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -892,27 +924,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1219,7 +1239,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,13 +1289,13 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="4"/>
@@ -1839,38 +1859,247 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="39" t="s">
         <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1749</v>
+      </c>
+      <c r="D3">
+        <v>1750</v>
+      </c>
+      <c r="E3">
+        <v>1751</v>
+      </c>
+      <c r="F3">
+        <v>1752</v>
+      </c>
+      <c r="G3">
+        <v>1753</v>
+      </c>
+      <c r="H3">
+        <v>1754</v>
+      </c>
+      <c r="I3">
+        <v>1755</v>
+      </c>
+      <c r="J3">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>137</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1757</v>
+      </c>
+      <c r="D4">
+        <v>1758</v>
+      </c>
+      <c r="E4">
+        <v>1759</v>
+      </c>
+      <c r="F4">
+        <v>1760</v>
+      </c>
+      <c r="G4">
+        <v>1761</v>
+      </c>
+      <c r="H4">
+        <v>1762</v>
+      </c>
+      <c r="I4">
+        <v>1763</v>
+      </c>
+      <c r="J4">
+        <v>1764</v>
+      </c>
+      <c r="K4">
+        <v>1765</v>
+      </c>
+      <c r="L4">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>235</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1767</v>
+      </c>
+      <c r="D5">
+        <v>1768</v>
+      </c>
+      <c r="E5">
+        <v>1769</v>
+      </c>
+      <c r="F5">
+        <v>1770</v>
+      </c>
+      <c r="G5">
+        <v>1771</v>
+      </c>
+      <c r="H5">
+        <v>1772</v>
+      </c>
+      <c r="I5">
+        <v>1773</v>
+      </c>
+      <c r="J5">
+        <v>1774</v>
+      </c>
+      <c r="K5">
+        <v>1775</v>
+      </c>
+      <c r="L5">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>333</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1777</v>
+      </c>
+      <c r="D6">
+        <v>1778</v>
+      </c>
+      <c r="E6">
+        <v>1779</v>
+      </c>
+      <c r="F6">
+        <v>1780</v>
+      </c>
+      <c r="G6">
+        <v>1781</v>
+      </c>
+      <c r="H6">
+        <v>1782</v>
+      </c>
+      <c r="I6">
+        <v>1783</v>
+      </c>
+      <c r="J6">
+        <v>1784</v>
+      </c>
+      <c r="K6">
+        <v>1785</v>
+      </c>
+      <c r="L6">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>431</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1787</v>
+      </c>
+      <c r="D7">
+        <v>1788</v>
+      </c>
+      <c r="E7">
+        <v>1789</v>
+      </c>
+      <c r="F7">
+        <v>1790</v>
+      </c>
+      <c r="G7">
+        <v>1791</v>
+      </c>
+      <c r="H7">
+        <v>1792</v>
+      </c>
+      <c r="I7">
+        <v>1793</v>
+      </c>
+      <c r="J7">
+        <v>1794</v>
       </c>
     </row>
   </sheetData>
@@ -1880,219 +2109,234 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" customWidth="1"/>
     <col min="25" max="25" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-    </row>
-    <row r="2" spans="1:19" s="54" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="53" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="44"/>
+    </row>
+    <row r="2" spans="1:21" s="41" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="I2" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="J2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="53" t="s">
+      <c r="T2" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="U2" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="G2" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="M2" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" s="53" t="s">
+    </row>
+    <row r="3" spans="1:21" s="58" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="N3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="O3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="P3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="R3" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="S3" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="T3" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="U3" s="58" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="R2" s="53" t="s">
-        <v>125</v>
-      </c>
-      <c r="S2" s="53" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="M3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="N3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="O3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="P3" s="55" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q3" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="R3" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="S3" s="55" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="K4" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="L4" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="M4" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="N4" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="56" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" s="56" t="s">
+      <c r="O4" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="P4" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="56" t="s">
+      <c r="Q4" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="R4" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="S4" s="43" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="56" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" s="56" t="s">
+      <c r="T4" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="N4" s="56" t="s">
+      <c r="U4" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="O4" s="56" t="s">
-        <v>158</v>
-      </c>
-      <c r="P4" s="56" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q4" s="56" t="s">
-        <v>160</v>
-      </c>
-      <c r="R4" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="S4" s="56" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="H6" s="4"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2102,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,52 +2363,57 @@
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="53" t="s">
+      <c r="A2" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="40" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
+      <c r="A3" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="A4" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2176,313 +2425,310 @@
   <dimension ref="A1:BK4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="27" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="56"/>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+    </row>
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
+      <c r="AQ3" s="49"/>
+      <c r="AR3" s="49"/>
+      <c r="AS3" s="49"/>
+      <c r="AT3" s="49"/>
+      <c r="AU3" s="49"/>
+      <c r="AV3" s="49"/>
+      <c r="AW3" s="49"/>
+      <c r="AX3" s="49"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="48" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-    </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC3" s="46"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="46"/>
-      <c r="AF3" s="46"/>
-      <c r="AG3" s="46"/>
-      <c r="AH3" s="46"/>
-      <c r="AI3" s="46"/>
-      <c r="AJ3" s="46"/>
-      <c r="AK3" s="46"/>
-      <c r="AL3" s="46"/>
-      <c r="AM3" s="47"/>
-      <c r="AN3" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="AO3" s="46"/>
-      <c r="AP3" s="46"/>
-      <c r="AQ3" s="46"/>
-      <c r="AR3" s="46"/>
-      <c r="AS3" s="46"/>
-      <c r="AT3" s="46"/>
-      <c r="AU3" s="46"/>
-      <c r="AV3" s="46"/>
-      <c r="AW3" s="46"/>
-      <c r="AX3" s="46"/>
-      <c r="AY3" s="47"/>
-      <c r="AZ3" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="BA3" s="46"/>
-      <c r="BB3" s="46"/>
-      <c r="BC3" s="46"/>
-      <c r="BD3" s="46"/>
-      <c r="BE3" s="46"/>
-      <c r="BF3" s="46"/>
-      <c r="BG3" s="46"/>
-      <c r="BH3" s="46"/>
-      <c r="BI3" s="46"/>
-      <c r="BJ3" s="46"/>
-      <c r="BK3" s="47"/>
+      <c r="BA3" s="49"/>
+      <c r="BB3" s="49"/>
+      <c r="BC3" s="49"/>
+      <c r="BD3" s="49"/>
+      <c r="BE3" s="49"/>
+      <c r="BF3" s="49"/>
+      <c r="BG3" s="49"/>
+      <c r="BH3" s="49"/>
+      <c r="BI3" s="49"/>
+      <c r="BJ3" s="49"/>
+      <c r="BK3" s="50"/>
     </row>
     <row r="4" spans="1:63" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="L4" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="P4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="Q4" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="T4" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="U4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="V4" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="W4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="X4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="L4" s="23" t="s">
+      <c r="Y4" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="Z4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="AA4" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="AB4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC4" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD4" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="AE4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG4" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ4" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM4" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="AP4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS4" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="AV4" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY4" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ4" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="BA4" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD4" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="BE4" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="U4" s="23" t="s">
+      <c r="BF4" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="BG4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="W4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="X4" s="23" t="s">
+      <c r="BI4" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="Y4" s="23" t="s">
+      <c r="BJ4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="Z4" s="23" t="s">
+      <c r="BK4" s="23" t="s">
         <v>79</v>
-      </c>
-      <c r="AA4" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="AD4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF4" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG4" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AH4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AI4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ4" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK4" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL4" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM4" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="AQ4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR4" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="AS4" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AT4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AU4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV4" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="AW4" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="AX4" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY4" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="AZ4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="BA4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="BB4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="BC4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="BD4" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="BE4" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="BF4" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="BG4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="BH4" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="BI4" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="BJ4" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="BK4" s="24" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2502,197 +2748,191 @@
   <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="39" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="39" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A1" s="56"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="48" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="50" t="s">
+      <c r="W3" s="51"/>
+      <c r="X3" s="51"/>
+      <c r="Y3" s="51"/>
+      <c r="Z3" s="51"/>
+      <c r="AA3" s="51"/>
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="49"/>
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51"/>
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51"/>
+      <c r="AJ3" s="51"/>
+      <c r="AK3" s="51"/>
+      <c r="AL3" s="51"/>
+      <c r="AM3" s="52"/>
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
       <c r="AQ3" s="4"/>
       <c r="AR3" s="4"/>
     </row>
-    <row r="4" spans="1:44" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="F4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="G4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="H4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="K4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="L4" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="O4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="P4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="Q4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="R4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Q4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" s="38" t="s">
+      <c r="S4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="S4" s="38" t="s">
+      <c r="T4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="T4" s="38" t="s">
+      <c r="U4" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="U4" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="V4" s="37" t="s">
+      <c r="V4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="W4" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="W4" s="38" t="s">
+      <c r="X4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="X4" s="38" t="s">
+      <c r="Y4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="Y4" s="38" t="s">
+      <c r="Z4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Z4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA4" s="38" t="s">
+      <c r="AB4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AB4" s="38" t="s">
+      <c r="AC4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="AC4" s="38" t="s">
+      <c r="AD4" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="AD4" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE4" s="38" t="s">
+      <c r="AE4" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF4" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="AF4" s="38" t="s">
+      <c r="AG4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="AG4" s="38" t="s">
+      <c r="AH4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="AH4" s="38" t="s">
+      <c r="AI4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="AI4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ4" s="38" t="s">
+      <c r="AK4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="AK4" s="38" t="s">
+      <c r="AL4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="AL4" s="38" t="s">
+      <c r="AM4" s="38" t="s">
         <v>79</v>
-      </c>
-      <c r="AM4" s="39" t="s">
-        <v>80</v>
       </c>
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
@@ -2701,9 +2941,6 @@
       <c r="AR4" s="4"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -2747,9 +2984,6 @@
       <c r="AR5" s="4"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2793,9 +3027,6 @@
       <c r="AR6" s="4"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -2839,9 +3070,6 @@
       <c r="AR7" s="4"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2885,9 +3113,6 @@
       <c r="AR8" s="4"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2931,9 +3156,6 @@
       <c r="AR9" s="4"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2977,9 +3199,6 @@
       <c r="AR10" s="4"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -3038,99 +3257,98 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="15" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="A1" s="56"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="44"/>
-    </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" s="23" t="s">
+      <c r="L4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="L4" s="23" t="s">
+      <c r="M4" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="N4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="O4" s="23" t="s">
         <v>79</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3146,115 +3364,109 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE36" sqref="AE36"/>
+      <selection activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A1" s="56"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
-      <c r="M3" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="49"/>
-    </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="57"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="51"/>
+      <c r="U3" s="52"/>
+    </row>
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="F4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="G4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="H4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="K4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="L4" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="O4" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="P4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="Q4" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="R4" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Q4" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" s="38" t="s">
+      <c r="S4" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="S4" s="38" t="s">
+      <c r="T4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="T4" s="38" t="s">
+      <c r="U4" s="38" t="s">
         <v>79</v>
-      </c>
-      <c r="U4" s="39" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3270,219 +3482,219 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" style="34" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="45" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="32">
+        <v>1</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="32">
+        <v>1</v>
+      </c>
+      <c r="C6" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="32">
+        <v>1.25</v>
+      </c>
+      <c r="C7" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="C8" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="32">
+        <v>1.75</v>
+      </c>
+      <c r="C9" s="32">
+        <v>1.3</v>
+      </c>
+      <c r="E9" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="33">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="32">
+        <v>1.35</v>
+      </c>
+      <c r="C10" s="32">
         <v>1</v>
       </c>
-      <c r="C5" s="33">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="C11" s="32">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="32">
+        <v>1.45</v>
+      </c>
+      <c r="C12" s="32">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B14" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="25"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="32">
+        <v>0.85</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="32">
         <v>1</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C19" s="32"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="32">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="33">
-        <v>1.25</v>
-      </c>
-      <c r="C7" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="C8" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="33">
-        <v>1.75</v>
-      </c>
-      <c r="C9" s="33">
-        <v>1.3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="33">
-        <v>1.35</v>
-      </c>
-      <c r="C10" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="33">
-        <v>1.45</v>
-      </c>
-      <c r="C11" s="33">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="33">
-        <v>1.45</v>
-      </c>
-      <c r="C12" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="36">
-        <v>0.95</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="26"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="33">
-        <v>0.85</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="34"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="33">
-        <v>1</v>
-      </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="33">
-        <v>1</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="35"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="33">
+      <c r="B22" s="32">
         <v>1.06</v>
       </c>
     </row>
@@ -3497,23 +3709,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>122</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="60"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>